<commit_message>
Add packages for well-formed project structure. Add ResultWriter class that write results in text file. Add wait for page loading method in Waiter class, create AvailableFilmsTest class that contains simple test. Add result.txt file. Create testng.xml for setup reportNg reporter in framework, modify pom.xml for reportNg well-work.
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -45,7 +45,7 @@
     <t>Харьков</t>
   </si>
   <si>
-    <t>30 июля, Сб</t>
+    <t>5 августа, Пт</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>